<commit_message>
update sim study to add no alarm and cases only
</commit_message>
<xml_diff>
--- a/simulation_study6/simParamsSummary.xlsx
+++ b/simulation_study6/simParamsSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ward-c\Documents\Postdoc\multipleDataBCM\simulation_study6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AABA73-00A5-488D-85B1-776D1F9201A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E575671C-CA84-4B5E-B4FD-E3B22D0EA44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4785" windowWidth="25440" windowHeight="15270" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
+    <workbookView xWindow="30612" yWindow="-204" windowWidth="30936" windowHeight="16776" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="24">
   <si>
     <t>IType</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>deltaD</t>
+  </si>
+  <si>
+    <t>probDetect</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564B3836-2B17-48DB-8114-869B4A6EAD37}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,7 +497,7 @@
     <col min="6" max="12" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -531,8 +534,11 @@
       <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -569,8 +575,11 @@
       <c r="L2" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
@@ -607,8 +616,11 @@
       <c r="L3" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -645,12 +657,15 @@
       <c r="L4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>

</xml_diff>